<commit_message>
fixed bug for Kenya values
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/WB-LGAF/WB-LGAF2016.xlsx
+++ b/Simple_XLS_Importer/data/WB-LGAF/WB-LGAF2016.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5785" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5788" uniqueCount="392">
   <si>
     <t>Panel</t>
   </si>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1857"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A1067" workbookViewId="0">
+      <selection activeCell="E1101" sqref="E1101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -16425,7 +16425,9 @@
       <c r="C1073" s="12">
         <v>2016</v>
       </c>
-      <c r="D1073" s="15"/>
+      <c r="D1073" s="15" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="1074" spans="1:4">
       <c r="A1074" s="12" t="s">
@@ -16563,7 +16565,9 @@
       <c r="C1083" s="12">
         <v>2016</v>
       </c>
-      <c r="D1083" s="15"/>
+      <c r="D1083" s="15" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="1084" spans="1:4">
       <c r="A1084" s="12" t="s">
@@ -16813,7 +16817,9 @@
       <c r="C1101" s="12">
         <v>2016</v>
       </c>
-      <c r="D1101" s="15"/>
+      <c r="D1101" s="15" t="s">
+        <v>261</v>
+      </c>
       <c r="E1101" s="12"/>
     </row>
     <row r="1102" spans="1:5">

</xml_diff>